<commit_message>
Add Custom DisplayFor for BusinessContacts with Bootstrap responsive Layout.
</commit_message>
<xml_diff>
--- a/LocalBusiness/Todo.xlsx
+++ b/LocalBusiness/Todo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="84">
   <si>
     <t>Priority</t>
   </si>
@@ -262,6 +262,18 @@
   </si>
   <si>
     <t>Display, Events, Schedule</t>
+  </si>
+  <si>
+    <t>Contacts Responsive Format</t>
+  </si>
+  <si>
+    <t>Events Responsive Format</t>
+  </si>
+  <si>
+    <t>Brands Responsive Format</t>
+  </si>
+  <si>
+    <t>Schedule Responsive Format</t>
   </si>
 </sst>
 </file>
@@ -437,151 +449,7 @@
     <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <font>
         <b/>
@@ -882,14 +750,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:H29" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:H38" totalsRowShown="0">
   <sortState ref="A2:H29">
     <sortCondition descending="1" ref="C1"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" name="Projectdependency _x000a_((low)1-(high)5)"/>
-    <tableColumn id="2" name="Effort _x000a_((low)1-(high)5)" dataDxfId="37"/>
-    <tableColumn id="8" name="Priority" dataDxfId="36">
+    <tableColumn id="2" name="Effort _x000a_((low)1-(high)5)" dataDxfId="25"/>
+    <tableColumn id="8" name="Priority" dataDxfId="24">
       <calculatedColumnFormula>(Tabelle1[[#This Row],[Projectdependency 
 ((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
 ((low)1-(high)5)]]))/2</calculatedColumnFormula>
@@ -1214,10 +1082,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:H367"/>
+  <dimension ref="A1:H376"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1278,7 +1146,7 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1451,7 +1319,7 @@
         <v>31</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1923,34 +1791,205 @@
       </c>
     </row>
     <row r="29" spans="1:8" s="12" customFormat="1">
-      <c r="A29"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29"/>
-      <c r="E29"/>
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" s="2">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" t="s">
+        <v>38</v>
+      </c>
       <c r="F29"/>
       <c r="G29"/>
-      <c r="H29"/>
-    </row>
-    <row r="30" spans="1:8" s="12" customFormat="1"/>
-    <row r="31" spans="1:8" s="12" customFormat="1"/>
-    <row r="32" spans="1:8" s="12" customFormat="1"/>
-    <row r="33" s="12" customFormat="1"/>
-    <row r="34" s="12" customFormat="1"/>
-    <row r="35" s="12" customFormat="1"/>
-    <row r="36" s="12" customFormat="1"/>
-    <row r="37" s="12" customFormat="1"/>
-    <row r="38" s="12" customFormat="1"/>
-    <row r="39" s="12" customFormat="1"/>
-    <row r="40" s="12" customFormat="1"/>
-    <row r="41" s="12" customFormat="1"/>
-    <row r="42" s="12" customFormat="1"/>
-    <row r="43" s="12" customFormat="1"/>
-    <row r="44" s="12" customFormat="1"/>
-    <row r="45" s="12" customFormat="1"/>
-    <row r="46" s="12" customFormat="1"/>
-    <row r="47" s="12" customFormat="1"/>
-    <row r="48" s="12" customFormat="1"/>
+      <c r="H29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="12" customFormat="1">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" s="2">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="12" customFormat="1">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" s="2">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>82</v>
+      </c>
+      <c r="E31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="12" customFormat="1">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" s="2">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="12" customFormat="1">
+      <c r="A33"/>
+      <c r="B33" s="2"/>
+      <c r="C33">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
+        <v>3</v>
+      </c>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+    </row>
+    <row r="34" spans="1:8" s="12" customFormat="1">
+      <c r="A34"/>
+      <c r="B34" s="2"/>
+      <c r="C34">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
+        <v>3</v>
+      </c>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+    </row>
+    <row r="35" spans="1:8" s="12" customFormat="1">
+      <c r="A35"/>
+      <c r="B35" s="2"/>
+      <c r="C35">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
+        <v>3</v>
+      </c>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+    </row>
+    <row r="36" spans="1:8" s="12" customFormat="1">
+      <c r="A36"/>
+      <c r="B36" s="2"/>
+      <c r="C36">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
+        <v>3</v>
+      </c>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+    </row>
+    <row r="37" spans="1:8" s="12" customFormat="1">
+      <c r="A37"/>
+      <c r="B37" s="2"/>
+      <c r="C37">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
+        <v>3</v>
+      </c>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+    </row>
+    <row r="38" spans="1:8" s="12" customFormat="1">
+      <c r="A38"/>
+      <c r="B38" s="2"/>
+      <c r="C38">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
+        <v>3</v>
+      </c>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+    </row>
+    <row r="39" spans="1:8" s="12" customFormat="1"/>
+    <row r="40" spans="1:8" s="12" customFormat="1"/>
+    <row r="41" spans="1:8" s="12" customFormat="1"/>
+    <row r="42" spans="1:8" s="12" customFormat="1"/>
+    <row r="43" spans="1:8" s="12" customFormat="1"/>
+    <row r="44" spans="1:8" s="12" customFormat="1"/>
+    <row r="45" spans="1:8" s="12" customFormat="1"/>
+    <row r="46" spans="1:8" s="12" customFormat="1"/>
+    <row r="47" spans="1:8" s="12" customFormat="1"/>
+    <row r="48" spans="1:8" s="12" customFormat="1"/>
     <row r="49" s="12" customFormat="1"/>
     <row r="50" s="12" customFormat="1"/>
     <row r="51" s="12" customFormat="1"/>
@@ -2360,54 +2399,144 @@
       <c r="G367" s="12"/>
       <c r="H367" s="12"/>
     </row>
+    <row r="368" spans="1:8">
+      <c r="A368" s="12"/>
+      <c r="B368" s="12"/>
+      <c r="C368" s="12"/>
+      <c r="D368" s="12"/>
+      <c r="E368" s="12"/>
+      <c r="F368" s="12"/>
+      <c r="G368" s="12"/>
+      <c r="H368" s="12"/>
+    </row>
+    <row r="369" spans="1:8">
+      <c r="A369" s="12"/>
+      <c r="B369" s="12"/>
+      <c r="C369" s="12"/>
+      <c r="D369" s="12"/>
+      <c r="E369" s="12"/>
+      <c r="F369" s="12"/>
+      <c r="G369" s="12"/>
+      <c r="H369" s="12"/>
+    </row>
+    <row r="370" spans="1:8">
+      <c r="A370" s="12"/>
+      <c r="B370" s="12"/>
+      <c r="C370" s="12"/>
+      <c r="D370" s="12"/>
+      <c r="E370" s="12"/>
+      <c r="F370" s="12"/>
+      <c r="G370" s="12"/>
+      <c r="H370" s="12"/>
+    </row>
+    <row r="371" spans="1:8">
+      <c r="A371" s="12"/>
+      <c r="B371" s="12"/>
+      <c r="C371" s="12"/>
+      <c r="D371" s="12"/>
+      <c r="E371" s="12"/>
+      <c r="F371" s="12"/>
+      <c r="G371" s="12"/>
+      <c r="H371" s="12"/>
+    </row>
+    <row r="372" spans="1:8">
+      <c r="A372" s="12"/>
+      <c r="B372" s="12"/>
+      <c r="C372" s="12"/>
+      <c r="D372" s="12"/>
+      <c r="E372" s="12"/>
+      <c r="F372" s="12"/>
+      <c r="G372" s="12"/>
+      <c r="H372" s="12"/>
+    </row>
+    <row r="373" spans="1:8">
+      <c r="A373" s="12"/>
+      <c r="B373" s="12"/>
+      <c r="C373" s="12"/>
+      <c r="D373" s="12"/>
+      <c r="E373" s="12"/>
+      <c r="F373" s="12"/>
+      <c r="G373" s="12"/>
+      <c r="H373" s="12"/>
+    </row>
+    <row r="374" spans="1:8">
+      <c r="A374" s="12"/>
+      <c r="B374" s="12"/>
+      <c r="C374" s="12"/>
+      <c r="D374" s="12"/>
+      <c r="E374" s="12"/>
+      <c r="F374" s="12"/>
+      <c r="G374" s="12"/>
+      <c r="H374" s="12"/>
+    </row>
+    <row r="375" spans="1:8">
+      <c r="A375" s="12"/>
+      <c r="B375" s="12"/>
+      <c r="C375" s="12"/>
+      <c r="D375" s="12"/>
+      <c r="E375" s="12"/>
+      <c r="F375" s="12"/>
+      <c r="G375" s="12"/>
+      <c r="H375" s="12"/>
+    </row>
+    <row r="376" spans="1:8">
+      <c r="A376" s="12"/>
+      <c r="B376" s="12"/>
+      <c r="C376" s="12"/>
+      <c r="D376" s="12"/>
+      <c r="E376" s="12"/>
+      <c r="F376" s="12"/>
+      <c r="G376" s="12"/>
+      <c r="H376" s="12"/>
+    </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A2:H367">
-    <cfRule type="expression" dxfId="35" priority="43">
+  <conditionalFormatting sqref="A2:H376">
+    <cfRule type="expression" dxfId="17" priority="43">
       <formula>$H2="Created"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="44">
+    <cfRule type="expression" dxfId="16" priority="44">
       <formula>$H2="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="45">
+    <cfRule type="expression" dxfId="15" priority="45">
       <formula>$H2="Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="46">
+    <cfRule type="expression" dxfId="14" priority="46">
       <formula>$H2="Implemented"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="47">
+    <cfRule type="expression" dxfId="13" priority="47">
       <formula>$H2="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2 A3:H367">
-    <cfRule type="expression" dxfId="30" priority="37">
+  <conditionalFormatting sqref="H2 A3:H376">
+    <cfRule type="expression" dxfId="12" priority="37">
       <formula>$H2="InWork"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:XFD357">
-    <cfRule type="expression" dxfId="29" priority="48">
-      <formula>$H30="Created"</formula>
+    <cfRule type="expression" dxfId="11" priority="48">
+      <formula>$H39="Created"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="49">
-      <formula>$H30="Done"</formula>
+    <cfRule type="expression" dxfId="10" priority="49">
+      <formula>$H39="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="50">
-      <formula>$H30="Ready"</formula>
+    <cfRule type="expression" dxfId="9" priority="50">
+      <formula>$H39="Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="51">
-      <formula>$H30="Implemented"</formula>
+    <cfRule type="expression" dxfId="8" priority="51">
+      <formula>$H39="Implemented"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="52">
-      <formula>$H30="Deprecated"</formula>
+    <cfRule type="expression" dxfId="7" priority="52">
+      <formula>$H39="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:XFD357">
-    <cfRule type="expression" dxfId="24" priority="63">
-      <formula>$H30="InWork"</formula>
+    <cfRule type="expression" dxfId="6" priority="63">
+      <formula>$H39="InWork"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H38">
       <formula1>statList</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>